<commit_message>
Added working code for Level2
</commit_message>
<xml_diff>
--- a/data/datacorr.xlsx
+++ b/data/datacorr.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="940" windowWidth="25040" windowHeight="14500" xr2:uid="{320A022A-14B1-7D42-A688-0F15D5749A71}"/>
+    <workbookView xWindow="560" yWindow="1020" windowWidth="25040" windowHeight="14500" xr2:uid="{320A022A-14B1-7D42-A688-0F15D5749A71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>AL</t>
   </si>
@@ -300,6 +300,18 @@
   </si>
   <si>
     <t>medianIncome</t>
+  </si>
+  <si>
+    <t>collegePlus</t>
+  </si>
+  <si>
+    <t>povertyAbove200</t>
+  </si>
+  <si>
+    <t>noHighSchoolGrad</t>
+  </si>
+  <si>
+    <t>hasHealthCare</t>
   </si>
 </sst>
 </file>
@@ -651,15 +663,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E24ED9-AA33-5E41-ACC1-2564483D95A1}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -667,13 +679,25 @@
         <v>89</v>
       </c>
       <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
         <v>90</v>
       </c>
-      <c r="D1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -681,13 +705,25 @@
         <v>1</v>
       </c>
       <c r="C2">
+        <v>42830</v>
+      </c>
+      <c r="D2">
         <v>5.9</v>
       </c>
-      <c r="D2">
-        <v>42830</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>59.6</v>
+      </c>
+      <c r="F2">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="G2">
+        <v>15.3</v>
+      </c>
+      <c r="H2">
+        <v>86.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -695,13 +731,25 @@
         <v>3</v>
       </c>
       <c r="C3">
+        <v>50068</v>
+      </c>
+      <c r="D3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D3">
-        <v>50068</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>61.2</v>
+      </c>
+      <c r="F3">
+        <v>23.9</v>
+      </c>
+      <c r="G3">
+        <v>13.9</v>
+      </c>
+      <c r="H3">
+        <v>85.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -709,13 +757,25 @@
         <v>5</v>
       </c>
       <c r="C4">
+        <v>41262</v>
+      </c>
+      <c r="D4">
         <v>6.7</v>
       </c>
-      <c r="D4">
-        <v>41262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>57.3</v>
+      </c>
+      <c r="F4">
+        <v>18.2</v>
+      </c>
+      <c r="G4">
+        <v>14.7</v>
+      </c>
+      <c r="H4">
+        <v>83.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -723,13 +783,25 @@
         <v>7</v>
       </c>
       <c r="C5">
+        <v>61933</v>
+      </c>
+      <c r="D5">
         <v>3.5</v>
       </c>
-      <c r="D5">
-        <v>61933</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>63.9</v>
+      </c>
+      <c r="F5">
+        <v>27.3</v>
+      </c>
+      <c r="G5">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="H5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -737,13 +809,25 @@
         <v>9</v>
       </c>
       <c r="C6">
+        <v>61303</v>
+      </c>
+      <c r="D6">
         <v>3.1</v>
       </c>
-      <c r="D6">
-        <v>61303</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>71</v>
+      </c>
+      <c r="F6">
+        <v>33.4</v>
+      </c>
+      <c r="G6">
+        <v>9.5</v>
+      </c>
+      <c r="H6">
+        <v>87.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -751,13 +835,25 @@
         <v>11</v>
       </c>
       <c r="C7">
+        <v>70048</v>
+      </c>
+      <c r="D7">
         <v>3.7</v>
       </c>
-      <c r="D7">
-        <v>70048</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="F7">
+        <v>32.9</v>
+      </c>
+      <c r="G7">
+        <v>9.9</v>
+      </c>
+      <c r="H7">
+        <v>91.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -765,13 +861,25 @@
         <v>13</v>
       </c>
       <c r="C8">
+        <v>59716</v>
+      </c>
+      <c r="D8">
         <v>5</v>
       </c>
-      <c r="D8">
-        <v>59716</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>72.5</v>
+      </c>
+      <c r="F8">
+        <v>26.1</v>
+      </c>
+      <c r="G8">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>91.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -779,13 +887,25 @@
         <v>15</v>
       </c>
       <c r="C9">
+        <v>71648</v>
+      </c>
+      <c r="D9">
         <v>2.6</v>
       </c>
-      <c r="D9">
-        <v>71648</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>68.5</v>
+      </c>
+      <c r="F9">
+        <v>49.1</v>
+      </c>
+      <c r="G9">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="H9">
+        <v>91.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -793,13 +913,25 @@
         <v>17</v>
       </c>
       <c r="C10">
+        <v>47463</v>
+      </c>
+      <c r="D10">
         <v>5.3</v>
       </c>
-      <c r="D10">
-        <v>47463</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>62.1</v>
+      </c>
+      <c r="F10">
+        <v>24.1</v>
+      </c>
+      <c r="G10">
+        <v>12.8</v>
+      </c>
+      <c r="H10">
+        <v>82.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -807,13 +939,25 @@
         <v>19</v>
       </c>
       <c r="C11">
+        <v>49321</v>
+      </c>
+      <c r="D11">
         <v>4.5</v>
       </c>
-      <c r="D11">
-        <v>49321</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>61.6</v>
+      </c>
+      <c r="F11">
+        <v>24.7</v>
+      </c>
+      <c r="G11">
+        <v>14.4</v>
+      </c>
+      <c r="H11">
+        <v>79.099999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -821,13 +965,25 @@
         <v>21</v>
       </c>
       <c r="C12">
+        <v>69592</v>
+      </c>
+      <c r="D12">
         <v>3.1</v>
       </c>
-      <c r="D12">
-        <v>69592</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="F12">
+        <v>27.3</v>
+      </c>
+      <c r="G12">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H12">
+        <v>91.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -835,13 +991,25 @@
         <v>23</v>
       </c>
       <c r="C13">
+        <v>47861</v>
+      </c>
+      <c r="D13">
         <v>3.7</v>
       </c>
-      <c r="D13">
-        <v>47861</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>61.8</v>
+      </c>
+      <c r="F13">
+        <v>22.4</v>
+      </c>
+      <c r="G13">
+        <v>9.9</v>
+      </c>
+      <c r="H13">
+        <v>83.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -849,13 +1017,25 @@
         <v>25</v>
       </c>
       <c r="C14">
+        <v>57444</v>
+      </c>
+      <c r="D14">
         <v>3.7</v>
       </c>
-      <c r="D14">
-        <v>57444</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>68.5</v>
+      </c>
+      <c r="F14">
+        <v>28.4</v>
+      </c>
+      <c r="G14">
+        <v>11.8</v>
+      </c>
+      <c r="H14">
+        <v>88.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -863,13 +1043,25 @@
         <v>27</v>
       </c>
       <c r="C15">
+        <v>49446</v>
+      </c>
+      <c r="D15">
         <v>5</v>
       </c>
-      <c r="D15">
-        <v>49446</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>65.3</v>
+      </c>
+      <c r="F15">
+        <v>20.8</v>
+      </c>
+      <c r="G15">
+        <v>11.6</v>
+      </c>
+      <c r="H15">
+        <v>85.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -877,13 +1069,25 @@
         <v>29</v>
       </c>
       <c r="C16">
+        <v>53712</v>
+      </c>
+      <c r="D16">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D16">
-        <v>53712</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="F16">
+        <v>23.4</v>
+      </c>
+      <c r="G16">
+        <v>7.9</v>
+      </c>
+      <c r="H16">
+        <v>92.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -891,13 +1095,25 @@
         <v>31</v>
       </c>
       <c r="C17">
+        <v>52504</v>
+      </c>
+      <c r="D17">
         <v>4.2</v>
       </c>
-      <c r="D17">
-        <v>52504</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>68</v>
+      </c>
+      <c r="F17">
+        <v>27</v>
+      </c>
+      <c r="G17">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H17">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -905,13 +1121,25 @@
         <v>33</v>
       </c>
       <c r="C18">
+        <v>42958</v>
+      </c>
+      <c r="D18">
         <v>6.8</v>
       </c>
-      <c r="D18">
-        <v>42958</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>60.2</v>
+      </c>
+      <c r="F18">
+        <v>19.3</v>
+      </c>
+      <c r="G18">
+        <v>15.5</v>
+      </c>
+      <c r="H18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -919,13 +1147,25 @@
         <v>35</v>
       </c>
       <c r="C19">
+        <v>44555</v>
+      </c>
+      <c r="D19">
         <v>5.2</v>
       </c>
-      <c r="D19">
-        <v>44555</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>59.7</v>
+      </c>
+      <c r="F19">
+        <v>19.8</v>
+      </c>
+      <c r="G19">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="H19">
+        <v>81.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -933,13 +1173,25 @@
         <v>37</v>
       </c>
       <c r="C20">
+        <v>73971</v>
+      </c>
+      <c r="D20">
         <v>3.2</v>
       </c>
-      <c r="D20">
-        <v>73971</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>76.2</v>
+      </c>
+      <c r="F20">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="G20">
+        <v>10.4</v>
+      </c>
+      <c r="H20">
+        <v>90.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -947,13 +1199,25 @@
         <v>39</v>
       </c>
       <c r="C21">
+        <v>69160</v>
+      </c>
+      <c r="D21">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D21">
-        <v>69160</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="F21">
+        <v>35.5</v>
+      </c>
+      <c r="G21">
+        <v>10.3</v>
+      </c>
+      <c r="H21">
+        <v>95.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -961,13 +1225,25 @@
         <v>41</v>
       </c>
       <c r="C22">
+        <v>49847</v>
+      </c>
+      <c r="D22">
         <v>5.2</v>
       </c>
-      <c r="D22">
-        <v>49847</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>65.3</v>
+      </c>
+      <c r="F22">
+        <v>23.4</v>
+      </c>
+      <c r="G22">
+        <v>10.1</v>
+      </c>
+      <c r="H22">
+        <v>89.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -975,13 +1251,25 @@
         <v>43</v>
       </c>
       <c r="C23">
+        <v>61481</v>
+      </c>
+      <c r="D23">
         <v>3.8</v>
       </c>
-      <c r="D23">
-        <v>61481</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="F23">
+        <v>29.6</v>
+      </c>
+      <c r="G23">
+        <v>7.4</v>
+      </c>
+      <c r="H23">
+        <v>92.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -989,13 +1277,25 @@
         <v>45</v>
       </c>
       <c r="C24">
+        <v>39680</v>
+      </c>
+      <c r="D24">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D24">
-        <v>39680</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>55.1</v>
+      </c>
+      <c r="F24">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="G24">
+        <v>17.2</v>
+      </c>
+      <c r="H24">
+        <v>81.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1003,13 +1303,25 @@
         <v>47</v>
       </c>
       <c r="C25">
+        <v>48363</v>
+      </c>
+      <c r="D25">
         <v>5.4</v>
       </c>
-      <c r="D25">
-        <v>48363</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>65</v>
+      </c>
+      <c r="F25">
+        <v>23.8</v>
+      </c>
+      <c r="G25">
+        <v>11.1</v>
+      </c>
+      <c r="H25">
+        <v>87.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1017,13 +1329,25 @@
         <v>49</v>
       </c>
       <c r="C26">
+        <v>52686</v>
+      </c>
+      <c r="D26">
         <v>3.8</v>
       </c>
-      <c r="D26">
-        <v>52686</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>69</v>
+      </c>
+      <c r="F26">
+        <v>25.8</v>
+      </c>
+      <c r="G26">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H26">
+        <v>87.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1031,13 +1355,25 @@
         <v>51</v>
       </c>
       <c r="C27">
+        <v>51450</v>
+      </c>
+      <c r="D27">
         <v>4.8</v>
       </c>
-      <c r="D27">
-        <v>51450</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>63.3</v>
+      </c>
+      <c r="F27">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G27">
+        <v>14.9</v>
+      </c>
+      <c r="H27">
+        <v>82.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1045,13 +1381,25 @@
         <v>53</v>
       </c>
       <c r="C28">
+        <v>66532</v>
+      </c>
+      <c r="D28">
         <v>3.8</v>
       </c>
-      <c r="D28">
-        <v>66532</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="F28">
+        <v>31</v>
+      </c>
+      <c r="G28">
+        <v>7.8</v>
+      </c>
+      <c r="H28">
+        <v>88.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1059,13 +1407,25 @@
         <v>55</v>
       </c>
       <c r="C29">
+        <v>71919</v>
+      </c>
+      <c r="D29">
         <v>4.2</v>
       </c>
-      <c r="D29">
-        <v>71919</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="F29">
+        <v>32.5</v>
+      </c>
+      <c r="G29">
+        <v>10.9</v>
+      </c>
+      <c r="H29">
+        <v>87.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1073,13 +1433,25 @@
         <v>57</v>
       </c>
       <c r="C30">
+        <v>44803</v>
+      </c>
+      <c r="D30">
         <v>4.2</v>
       </c>
-      <c r="D30">
-        <v>44803</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <v>56.5</v>
+      </c>
+      <c r="F30">
+        <v>22.8</v>
+      </c>
+      <c r="G30">
+        <v>15.8</v>
+      </c>
+      <c r="H30">
+        <v>84.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1087,13 +1459,25 @@
         <v>59</v>
       </c>
       <c r="C31">
+        <v>58878</v>
+      </c>
+      <c r="D31">
         <v>3.8</v>
       </c>
-      <c r="D31">
-        <v>58878</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>67.2</v>
+      </c>
+      <c r="F31">
+        <v>30.4</v>
+      </c>
+      <c r="G31">
+        <v>14.3</v>
+      </c>
+      <c r="H31">
+        <v>87.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -1101,13 +1485,25 @@
         <v>61</v>
       </c>
       <c r="C32">
+        <v>46556</v>
+      </c>
+      <c r="D32">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D32">
-        <v>46556</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <v>61.4</v>
+      </c>
+      <c r="F32">
+        <v>24.3</v>
+      </c>
+      <c r="G32">
+        <v>13.6</v>
+      </c>
+      <c r="H32">
+        <v>83.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -1115,13 +1511,25 @@
         <v>63</v>
       </c>
       <c r="C33">
+        <v>49308</v>
+      </c>
+      <c r="D33">
         <v>5.4</v>
       </c>
-      <c r="D33">
-        <v>49308</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33">
+        <v>66</v>
+      </c>
+      <c r="F33">
+        <v>22.8</v>
+      </c>
+      <c r="G33">
+        <v>10.6</v>
+      </c>
+      <c r="H33">
+        <v>89.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -1129,13 +1537,25 @@
         <v>65</v>
       </c>
       <c r="C34">
+        <v>47529</v>
+      </c>
+      <c r="D34">
         <v>5.5</v>
       </c>
-      <c r="D34">
-        <v>47529</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34">
+        <v>62.2</v>
+      </c>
+      <c r="F34">
+        <v>21</v>
+      </c>
+      <c r="G34">
+        <v>12.7</v>
+      </c>
+      <c r="H34">
+        <v>86.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -1143,13 +1563,25 @@
         <v>67</v>
       </c>
       <c r="C35">
+        <v>51075</v>
+      </c>
+      <c r="D35">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D35">
-        <v>51075</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <v>63.2</v>
+      </c>
+      <c r="F35">
+        <v>26.8</v>
+      </c>
+      <c r="G35">
+        <v>10.3</v>
+      </c>
+      <c r="H35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -1157,13 +1589,25 @@
         <v>69</v>
       </c>
       <c r="C36">
+        <v>53234</v>
+      </c>
+      <c r="D36">
         <v>4.8</v>
       </c>
-      <c r="D36">
-        <v>53234</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36">
+        <v>69.3</v>
+      </c>
+      <c r="F36">
+        <v>25.1</v>
+      </c>
+      <c r="G36">
+        <v>10.6</v>
+      </c>
+      <c r="H36">
+        <v>89.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1171,13 +1615,25 @@
         <v>71</v>
       </c>
       <c r="C37">
+        <v>54891</v>
+      </c>
+      <c r="D37">
         <v>4.3</v>
       </c>
-      <c r="D37">
-        <v>54891</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="F37">
+        <v>27.9</v>
+      </c>
+      <c r="G37">
+        <v>14.2</v>
+      </c>
+      <c r="H37">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1185,13 +1641,25 @@
         <v>73</v>
       </c>
       <c r="C38">
+        <v>45238</v>
+      </c>
+      <c r="D38">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D38">
-        <v>45238</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>60.8</v>
+      </c>
+      <c r="F38">
+        <v>22.5</v>
+      </c>
+      <c r="G38">
+        <v>13.9</v>
+      </c>
+      <c r="H38">
+        <v>82.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -1199,13 +1667,25 @@
         <v>75</v>
       </c>
       <c r="C39">
+        <v>44361</v>
+      </c>
+      <c r="D39">
         <v>5.7</v>
       </c>
-      <c r="D39">
-        <v>44361</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>60.2</v>
+      </c>
+      <c r="F39">
+        <v>21.5</v>
+      </c>
+      <c r="G39">
+        <v>14.2</v>
+      </c>
+      <c r="H39">
+        <v>85.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -1213,13 +1693,25 @@
         <v>77</v>
       </c>
       <c r="C40">
+        <v>53035</v>
+      </c>
+      <c r="D40">
         <v>3.7</v>
       </c>
-      <c r="D40">
-        <v>53035</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <v>62</v>
+      </c>
+      <c r="F40">
+        <v>23.5</v>
+      </c>
+      <c r="G40">
+        <v>17.8</v>
+      </c>
+      <c r="H40">
+        <v>75.099999999999994</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -1227,13 +1719,25 @@
         <v>79</v>
       </c>
       <c r="C41">
+        <v>60922</v>
+      </c>
+      <c r="D41">
         <v>2.9</v>
       </c>
-      <c r="D41">
-        <v>60922</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="F41">
+        <v>25.8</v>
+      </c>
+      <c r="G41">
+        <v>8.6</v>
+      </c>
+      <c r="H41">
+        <v>86.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1241,13 +1745,25 @@
         <v>81</v>
       </c>
       <c r="C42">
+        <v>64902</v>
+      </c>
+      <c r="D42">
         <v>4.2</v>
       </c>
-      <c r="D42">
-        <v>64902</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="F42">
+        <v>31.7</v>
+      </c>
+      <c r="G42">
+        <v>11.5</v>
+      </c>
+      <c r="H42">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -1255,13 +1771,25 @@
         <v>83</v>
       </c>
       <c r="C43">
+        <v>61366</v>
+      </c>
+      <c r="D43">
         <v>3.8</v>
       </c>
-      <c r="D43">
-        <v>61366</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="F43">
+        <v>28.7</v>
+      </c>
+      <c r="G43">
+        <v>9.6</v>
+      </c>
+      <c r="H43">
+        <v>89.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -1269,13 +1797,25 @@
         <v>85</v>
       </c>
       <c r="C44">
+        <v>52622</v>
+      </c>
+      <c r="D44">
         <v>3.7</v>
       </c>
-      <c r="D44">
-        <v>52622</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44">
+        <v>69.5</v>
+      </c>
+      <c r="F44">
+        <v>24.3</v>
+      </c>
+      <c r="G44">
+        <v>8.6</v>
+      </c>
+      <c r="H44">
+        <v>91.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -1283,10 +1823,22 @@
         <v>87</v>
       </c>
       <c r="C45">
+        <v>18928</v>
+      </c>
+      <c r="D45">
         <v>5.3</v>
       </c>
-      <c r="D45">
-        <v>18928</v>
+      <c r="E45">
+        <v>26.3</v>
+      </c>
+      <c r="F45">
+        <v>29.4</v>
+      </c>
+      <c r="G45">
+        <v>26.2</v>
+      </c>
+      <c r="H45">
+        <v>94.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the data set and updated code to reflect that. Updated Readme
</commit_message>
<xml_diff>
--- a/data/datacorr.xlsx
+++ b/data/datacorr.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>AL</t>
   </si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>hasHealthCare</t>
+  </si>
+  <si>
+    <t>hasCancer</t>
+  </si>
+  <si>
+    <t>hasDiabetes</t>
   </si>
 </sst>
 </file>
@@ -663,15 +669,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E24ED9-AA33-5E41-ACC1-2564483D95A1}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -696,8 +706,14 @@
       <c r="H1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -722,8 +738,14 @@
       <c r="H2">
         <v>86.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <v>12.9</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -748,8 +770,14 @@
       <c r="H3">
         <v>85.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>10.1</v>
+      </c>
+      <c r="J3">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -774,8 +802,14 @@
       <c r="H4">
         <v>83.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>12.8</v>
+      </c>
+      <c r="J4">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -800,8 +834,14 @@
       <c r="H5">
         <v>85.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <v>10.3</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -826,8 +866,14 @@
       <c r="H6">
         <v>87.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <v>7.3</v>
+      </c>
+      <c r="J6">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -852,8 +898,14 @@
       <c r="H7">
         <v>91.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J7">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -878,8 +930,14 @@
       <c r="H8">
         <v>91.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <v>11.1</v>
+      </c>
+      <c r="J8">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -904,8 +962,14 @@
       <c r="H9">
         <v>91.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <v>8.4</v>
+      </c>
+      <c r="J9">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -930,8 +994,14 @@
       <c r="H10">
         <v>82.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <v>11.2</v>
+      </c>
+      <c r="J10">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -956,8 +1026,14 @@
       <c r="H11">
         <v>79.099999999999994</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <v>11.6</v>
+      </c>
+      <c r="J11">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -982,8 +1058,14 @@
       <c r="H12">
         <v>91.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J12">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1008,8 +1090,14 @@
       <c r="H13">
         <v>83.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <v>7.6</v>
+      </c>
+      <c r="J13">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1034,8 +1122,14 @@
       <c r="H14">
         <v>88.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <v>10.1</v>
+      </c>
+      <c r="J14">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1060,8 +1154,14 @@
       <c r="H15">
         <v>85.3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <v>10.7</v>
+      </c>
+      <c r="J15">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1086,8 +1186,14 @@
       <c r="H16">
         <v>92.3</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <v>9.5</v>
+      </c>
+      <c r="J16">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1112,8 +1218,14 @@
       <c r="H17">
         <v>85.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <v>10.3</v>
+      </c>
+      <c r="J17">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1138,8 +1250,14 @@
       <c r="H18">
         <v>90</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <v>12.5</v>
+      </c>
+      <c r="J18">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1164,8 +1282,14 @@
       <c r="H19">
         <v>81.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <v>11.3</v>
+      </c>
+      <c r="J19">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1190,8 +1314,14 @@
       <c r="H20">
         <v>90.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <v>10.1</v>
+      </c>
+      <c r="J20">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1216,8 +1346,14 @@
       <c r="H21">
         <v>95.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="J21">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1242,8 +1378,14 @@
       <c r="H22">
         <v>89.7</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22">
+        <v>10.4</v>
+      </c>
+      <c r="J22">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1268,8 +1410,14 @@
       <c r="H23">
         <v>92.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23">
+        <v>8.1</v>
+      </c>
+      <c r="J23">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1294,8 +1442,14 @@
       <c r="H24">
         <v>81.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24">
+        <v>13</v>
+      </c>
+      <c r="J24">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1320,8 +1474,14 @@
       <c r="H25">
         <v>87.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25">
+        <v>11.1</v>
+      </c>
+      <c r="J25">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1346,8 +1506,14 @@
       <c r="H26">
         <v>87.7</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J26">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1372,8 +1538,14 @@
       <c r="H27">
         <v>82.9</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27">
+        <v>9.6</v>
+      </c>
+      <c r="J27">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1398,8 +1570,14 @@
       <c r="H28">
         <v>88.6</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1424,8 +1602,14 @@
       <c r="H29">
         <v>87.6</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="J29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1450,8 +1634,14 @@
       <c r="H30">
         <v>84.6</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30">
+        <v>11.5</v>
+      </c>
+      <c r="J30">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1476,8 +1666,14 @@
       <c r="H31">
         <v>87.7</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31">
+        <v>10</v>
+      </c>
+      <c r="J31">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -1502,8 +1698,14 @@
       <c r="H32">
         <v>83.9</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32">
+        <v>10.8</v>
+      </c>
+      <c r="J32">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -1528,8 +1730,14 @@
       <c r="H33">
         <v>89.8</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33">
+        <v>11.7</v>
+      </c>
+      <c r="J33">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -1554,8 +1762,14 @@
       <c r="H34">
         <v>86.1</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34">
+        <v>12</v>
+      </c>
+      <c r="J34">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -1580,8 +1794,14 @@
       <c r="H35">
         <v>89</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35">
+        <v>9</v>
+      </c>
+      <c r="J35">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -1606,8 +1826,14 @@
       <c r="H36">
         <v>89.9</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36">
+        <v>11.2</v>
+      </c>
+      <c r="J36">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1632,8 +1858,14 @@
       <c r="H37">
         <v>92</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37">
+        <v>9.5</v>
+      </c>
+      <c r="J37">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1658,8 +1890,14 @@
       <c r="H38">
         <v>82.9</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38">
+        <v>12</v>
+      </c>
+      <c r="J38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -1684,8 +1922,14 @@
       <c r="H39">
         <v>85.8</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39">
+        <v>13</v>
+      </c>
+      <c r="J39">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -1710,8 +1954,14 @@
       <c r="H40">
         <v>75.099999999999994</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40">
+        <v>11</v>
+      </c>
+      <c r="J40">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -1736,8 +1986,14 @@
       <c r="H41">
         <v>86.1</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41">
+        <v>7.1</v>
+      </c>
+      <c r="J41">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1762,8 +2018,14 @@
       <c r="H42">
         <v>87</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="J42">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -1788,8 +2050,14 @@
       <c r="H43">
         <v>89.3</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43">
+        <v>8.9</v>
+      </c>
+      <c r="J43">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -1814,8 +2082,14 @@
       <c r="H44">
         <v>91.5</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44">
+        <v>9</v>
+      </c>
+      <c r="J44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -1839,6 +2113,12 @@
       </c>
       <c r="H45">
         <v>94.1</v>
+      </c>
+      <c r="I45">
+        <v>15.7</v>
+      </c>
+      <c r="J45">
+        <v>4.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>